<commit_message>
no longer changes the role of a locked account
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 2 Access Matrix.xlsx
+++ b/CSSECDV - Case Study 2 Access Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\cpusched\CSSECDV-Case-Study-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CSSECDV\CSSECDV-Case-Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F674B3F-4A68-4E8F-B582-C7B5F1A85B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9709CC02-362E-49C5-8298-802F99829BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="885" windowWidth="29040" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
   <si>
     <t>ACCESS MATRIX</t>
   </si>
@@ -414,22 +414,6 @@
   </si>
   <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t>sanitization - replace symbols to unicode
-reject known bad - disallow symbols (",',&gt;,&lt;)
-hashing - Bcrypt with salt</t>
-  </si>
-  <si>
-    <t>sanitization - replace symbols to unicode
-min length
-max length
-disallow symbols reject known bad - disallow symbols (",',&gt;,&lt;)
-hashing - Bcrypt with salt</t>
-  </si>
-  <si>
-    <t>sql injection
-denial of service - logs</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -507,7 +491,11 @@
     <t>logs table</t>
   </si>
   <si>
-    <t>Session timeout was implemented where is the user has no actions for 10 minutes, they will be logged out and redirected to the login page.</t>
+    <t>Session timeout was implemented where is the user has no actions for 15 minutes, they will be logged out and redirected to the login page.</t>
+  </si>
+  <si>
+    <t>sql injection
+weak user credentials</t>
   </si>
 </sst>
 </file>
@@ -1200,26 +1188,26 @@
   <dimension ref="A1:CY19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="12" width="20.85546875" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="103" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="12" width="20.88671875" customWidth="1"/>
+    <col min="13" max="13" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="103" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="34" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" s="34" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:103" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1233,34 +1221,34 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>17</v>
@@ -1530,7 +1518,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1625,7 @@
       <c r="CX3" s="7"/>
       <c r="CY3" s="8"/>
     </row>
-    <row r="4" spans="1:103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
@@ -1744,7 +1732,7 @@
       <c r="CX4" s="7"/>
       <c r="CY4" s="8"/>
     </row>
-    <row r="5" spans="1:103" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:103" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -1756,7 +1744,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1853,7 +1841,7 @@
       <c r="CX5" s="7"/>
       <c r="CY5" s="8"/>
     </row>
-    <row r="6" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
@@ -1962,7 +1950,7 @@
       <c r="CX6" s="7"/>
       <c r="CY6" s="8"/>
     </row>
-    <row r="7" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
@@ -2071,7 +2059,7 @@
       <c r="CX7" s="7"/>
       <c r="CY7" s="8"/>
     </row>
-    <row r="8" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:103" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2166,7 @@
       <c r="CX8" s="10"/>
       <c r="CY8" s="12"/>
     </row>
-    <row r="9" spans="1:103" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -2283,7 +2271,7 @@
       <c r="CX9" s="23"/>
       <c r="CY9" s="23"/>
     </row>
-    <row r="10" spans="1:103" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:103" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>106</v>
       </c>
@@ -2294,37 +2282,37 @@
         <v>111</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="J10" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="K10" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="I10" s="28" t="s">
+      <c r="L10" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="N10" s="28" t="s">
         <v>137</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="N10" s="28" t="s">
-        <v>140</v>
       </c>
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
@@ -2416,7 +2404,7 @@
       <c r="CX10" s="28"/>
       <c r="CY10" s="28"/>
     </row>
-    <row r="11" spans="1:103" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:103" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
         <v>107</v>
       </c>
@@ -2529,12 +2517,12 @@
       <c r="CX11" s="25"/>
       <c r="CY11" s="25"/>
     </row>
-    <row r="12" spans="1:103" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:103" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>113</v>
@@ -2658,16 +2646,12 @@
       <c r="CX12" s="28"/>
       <c r="CY12" s="28"/>
     </row>
-    <row r="13" spans="1:103" ht="99.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:103" ht="99.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>116</v>
-      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="25" t="s">
         <v>115</v>
       </c>
@@ -2779,7 +2763,7 @@
       <c r="CX13" s="25"/>
       <c r="CY13" s="25"/>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -2884,13 +2868,13 @@
       <c r="CX14" s="23"/>
       <c r="CY14" s="23"/>
     </row>
-    <row r="15" spans="1:103" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:103" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -2993,22 +2977,22 @@
       <c r="CX15" s="33"/>
       <c r="CY15" s="33"/>
     </row>
-    <row r="16" spans="1:103" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:103" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>